<commit_message>
DOC: Add test scripts to README file
</commit_message>
<xml_diff>
--- a/documentation/tests/test-about-page.xlsx
+++ b/documentation/tests/test-about-page.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="35">
   <si>
     <t xml:space="preserve">Test  ID</t>
   </si>
@@ -194,8 +194,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -374,7 +375,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -475,11 +476,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -611,7 +608,7 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6:J11"/>
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -746,34 +743,38 @@
         <v>21</v>
       </c>
       <c r="F6" s="16"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26" t="str">
+      <c r="G6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="I6" s="25" t="str">
         <f aca="false">IF(G6=E6,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J6" s="26"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J6" s="25"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
     </row>
     <row r="7" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="22"/>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
       <c r="D7" s="24"/>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="26" t="str">
+      <c r="F7" s="27"/>
+      <c r="G7" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="27"/>
+      <c r="I7" s="25" t="str">
         <f aca="false">IF(G7=E7,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J7" s="26"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
     </row>
     <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="22"/>
@@ -784,53 +785,59 @@
         <v>23</v>
       </c>
       <c r="F8" s="16"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="26" t="str">
+      <c r="G8" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="I8" s="25" t="str">
         <f aca="false">IF(G8=E8,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J8" s="25"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="24"/>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="26" t="str">
+      <c r="F9" s="27"/>
+      <c r="G9" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="27"/>
+      <c r="I9" s="25" t="str">
         <f aca="false">IF(G9=E9,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J9" s="26"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J9" s="25"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="24"/>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="26" t="str">
+      <c r="F10" s="27"/>
+      <c r="G10" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="27"/>
+      <c r="I10" s="25" t="str">
         <f aca="false">IF(G10=E10,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J10" s="26"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J10" s="25"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
     </row>
     <row r="11" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="n">
@@ -847,15 +854,17 @@
         <v>28</v>
       </c>
       <c r="F11" s="23"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="26" t="str">
+      <c r="G11" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="23"/>
+      <c r="I11" s="25" t="str">
         <f aca="false">IF(G11=E11,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J11" s="26"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J11" s="25"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9"/>
@@ -872,64 +881,64 @@
       <c r="L12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="29"/>
+      <c r="A13" s="28"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="32" t="s">
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="34"/>
+      <c r="H14" s="33"/>
       <c r="I14" s="6"/>
       <c r="J14" s="7"/>
       <c r="L14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31" t="s">
+      <c r="B15" s="29"/>
+      <c r="C15" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="32" t="s">
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="35" t="s">
+      <c r="G15" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="35"/>
+      <c r="H15" s="34"/>
       <c r="I15" s="11"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="31" t="s">
+      <c r="B16" s="29"/>
+      <c r="C16" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32" t="s">
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="36"/>
-      <c r="H16" s="37"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="36"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
@@ -994,34 +1003,38 @@
         <v>21</v>
       </c>
       <c r="F19" s="16"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="26" t="str">
+      <c r="G19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="16"/>
+      <c r="I19" s="25" t="str">
         <f aca="false">IF(G19=E19,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J19" s="26"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J19" s="25"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
     </row>
     <row r="20" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
       <c r="C20" s="23"/>
       <c r="D20" s="24"/>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="26" t="str">
+      <c r="F20" s="27"/>
+      <c r="G20" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="27"/>
+      <c r="I20" s="25" t="str">
         <f aca="false">IF(G20=E20,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J20" s="26"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J20" s="25"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
     </row>
     <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="22"/>
@@ -1032,53 +1045,59 @@
         <v>23</v>
       </c>
       <c r="F21" s="16"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="26" t="str">
+      <c r="G21" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="16"/>
+      <c r="I21" s="25" t="str">
         <f aca="false">IF(G21=E21,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J21" s="26"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J21" s="25"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="22"/>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
       <c r="D22" s="24"/>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="26" t="str">
+      <c r="F22" s="27"/>
+      <c r="G22" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="27"/>
+      <c r="I22" s="25" t="str">
         <f aca="false">IF(G22=E22,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J22" s="26"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J22" s="25"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="22"/>
       <c r="B23" s="23"/>
       <c r="C23" s="23"/>
       <c r="D23" s="24"/>
-      <c r="E23" s="28" t="s">
+      <c r="E23" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="28"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="26" t="str">
+      <c r="F23" s="27"/>
+      <c r="G23" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="27"/>
+      <c r="I23" s="25" t="str">
         <f aca="false">IF(G23=E23,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J23" s="26"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J23" s="25"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
     </row>
     <row r="24" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="22" t="n">
@@ -1095,15 +1114,17 @@
         <v>28</v>
       </c>
       <c r="F24" s="23"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="26" t="str">
+      <c r="G24" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="23"/>
+      <c r="I24" s="25" t="str">
         <f aca="false">IF(G24=E24,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J24" s="26"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J24" s="25"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
     </row>
     <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1224,7 +1245,7 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6:J11"/>
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1333,10 +1354,10 @@
         <v>16</v>
       </c>
       <c r="H5" s="20"/>
-      <c r="I5" s="38" t="s">
+      <c r="I5" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="38"/>
+      <c r="J5" s="37"/>
       <c r="K5" s="18" t="s">
         <v>18</v>
       </c>
@@ -1357,34 +1378,38 @@
         <v>21</v>
       </c>
       <c r="F6" s="16"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26" t="str">
+      <c r="G6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="I6" s="25" t="str">
         <f aca="false">IF(G6=E6,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J6" s="26"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J6" s="25"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
     </row>
     <row r="7" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="22"/>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
       <c r="D7" s="24"/>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="26" t="str">
+      <c r="F7" s="27"/>
+      <c r="G7" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="27"/>
+      <c r="I7" s="25" t="str">
         <f aca="false">IF(G7=E7,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J7" s="26"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
     </row>
     <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="22"/>
@@ -1395,53 +1420,59 @@
         <v>23</v>
       </c>
       <c r="F8" s="16"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="26" t="str">
+      <c r="G8" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="I8" s="25" t="str">
         <f aca="false">IF(G8=E8,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J8" s="25"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="24"/>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="26" t="str">
+      <c r="F9" s="27"/>
+      <c r="G9" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="27"/>
+      <c r="I9" s="25" t="str">
         <f aca="false">IF(G9=E9,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J9" s="26"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J9" s="25"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="24"/>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="26" t="str">
+      <c r="F10" s="27"/>
+      <c r="G10" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="27"/>
+      <c r="I10" s="25" t="str">
         <f aca="false">IF(G10=E10,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J10" s="26"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J10" s="25"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
     </row>
     <row r="11" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="n">
@@ -1458,78 +1489,80 @@
         <v>28</v>
       </c>
       <c r="F11" s="23"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="26" t="str">
+      <c r="G11" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="23"/>
+      <c r="I11" s="25" t="str">
         <f aca="false">IF(G11=E11,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J11" s="26"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J11" s="25"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="29"/>
+      <c r="A12" s="28"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="29"/>
+      <c r="A13" s="28"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="32" t="s">
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="34"/>
+      <c r="H14" s="33"/>
       <c r="I14" s="6"/>
       <c r="J14" s="7"/>
       <c r="L14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31" t="s">
+      <c r="B15" s="29"/>
+      <c r="C15" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="32" t="s">
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="35" t="s">
+      <c r="G15" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="35"/>
+      <c r="H15" s="34"/>
       <c r="I15" s="11"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="31" t="s">
+      <c r="B16" s="29"/>
+      <c r="C16" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32" t="s">
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="36"/>
-      <c r="H16" s="37"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="36"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
@@ -1570,10 +1603,10 @@
         <v>16</v>
       </c>
       <c r="H18" s="20"/>
-      <c r="I18" s="38" t="s">
+      <c r="I18" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="38"/>
+      <c r="J18" s="37"/>
       <c r="K18" s="18" t="s">
         <v>18</v>
       </c>
@@ -1594,34 +1627,38 @@
         <v>21</v>
       </c>
       <c r="F19" s="16"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="26" t="str">
+      <c r="G19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="16"/>
+      <c r="I19" s="25" t="str">
         <f aca="false">IF(G19=E19,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J19" s="26"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J19" s="25"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
     </row>
     <row r="20" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
       <c r="C20" s="23"/>
       <c r="D20" s="24"/>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="26" t="str">
+      <c r="F20" s="27"/>
+      <c r="G20" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="27"/>
+      <c r="I20" s="25" t="str">
         <f aca="false">IF(G20=E20,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J20" s="26"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J20" s="25"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
     </row>
     <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="22"/>
@@ -1632,53 +1669,59 @@
         <v>23</v>
       </c>
       <c r="F21" s="16"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="26" t="str">
+      <c r="G21" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="16"/>
+      <c r="I21" s="25" t="str">
         <f aca="false">IF(G21=E21,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J21" s="26"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J21" s="25"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="22"/>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
       <c r="D22" s="24"/>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="26" t="str">
+      <c r="F22" s="27"/>
+      <c r="G22" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="27"/>
+      <c r="I22" s="25" t="str">
         <f aca="false">IF(G22=E22,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J22" s="26"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J22" s="25"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="22"/>
       <c r="B23" s="23"/>
       <c r="C23" s="23"/>
       <c r="D23" s="24"/>
-      <c r="E23" s="28" t="s">
+      <c r="E23" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="28"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="26" t="str">
+      <c r="F23" s="27"/>
+      <c r="G23" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="27"/>
+      <c r="I23" s="25" t="str">
         <f aca="false">IF(G23=E23,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J23" s="26"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J23" s="25"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
     </row>
     <row r="24" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="22" t="n">
@@ -1695,15 +1738,17 @@
         <v>28</v>
       </c>
       <c r="F24" s="23"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="26" t="str">
+      <c r="G24" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="23"/>
+      <c r="I24" s="25" t="str">
         <f aca="false">IF(G24=E24,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J24" s="26"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J24" s="25"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
     </row>
     <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1828,7 +1873,7 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6:J11"/>
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1937,10 +1982,10 @@
         <v>16</v>
       </c>
       <c r="H5" s="20"/>
-      <c r="I5" s="38" t="s">
+      <c r="I5" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="38"/>
+      <c r="J5" s="37"/>
       <c r="K5" s="18" t="s">
         <v>18</v>
       </c>
@@ -1961,34 +2006,38 @@
         <v>21</v>
       </c>
       <c r="F6" s="16"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26" t="str">
+      <c r="G6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="I6" s="25" t="str">
         <f aca="false">IF(G6=E6,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J6" s="26"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J6" s="25"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
     </row>
     <row r="7" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="22"/>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
       <c r="D7" s="24"/>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="26" t="str">
+      <c r="F7" s="27"/>
+      <c r="G7" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="27"/>
+      <c r="I7" s="25" t="str">
         <f aca="false">IF(G7=E7,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J7" s="26"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
     </row>
     <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="22"/>
@@ -1999,53 +2048,59 @@
         <v>23</v>
       </c>
       <c r="F8" s="16"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="26" t="str">
+      <c r="G8" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="I8" s="25" t="str">
         <f aca="false">IF(G8=E8,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J8" s="25"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="24"/>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="26" t="str">
+      <c r="F9" s="27"/>
+      <c r="G9" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="27"/>
+      <c r="I9" s="25" t="str">
         <f aca="false">IF(G9=E9,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J9" s="26"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J9" s="25"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="24"/>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="26" t="str">
+      <c r="F10" s="27"/>
+      <c r="G10" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="27"/>
+      <c r="I10" s="25" t="str">
         <f aca="false">IF(G10=E10,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J10" s="26"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J10" s="25"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
     </row>
     <row r="11" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="n">
@@ -2062,15 +2117,17 @@
         <v>28</v>
       </c>
       <c r="F11" s="23"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="26" t="str">
+      <c r="G11" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="23"/>
+      <c r="I11" s="25" t="str">
         <f aca="false">IF(G11=E11,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J11" s="26"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J11" s="25"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9"/>
@@ -2087,64 +2144,64 @@
       <c r="L12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="29"/>
+      <c r="A13" s="28"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="32" t="s">
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="34"/>
+      <c r="H14" s="33"/>
       <c r="I14" s="6"/>
       <c r="J14" s="7"/>
       <c r="L14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31" t="s">
+      <c r="B15" s="29"/>
+      <c r="C15" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="32" t="s">
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="35" t="s">
+      <c r="G15" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="35"/>
+      <c r="H15" s="34"/>
       <c r="I15" s="11"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="31" t="s">
+      <c r="B16" s="29"/>
+      <c r="C16" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32" t="s">
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="36"/>
-      <c r="H16" s="37"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="36"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
@@ -2185,10 +2242,10 @@
         <v>16</v>
       </c>
       <c r="H18" s="20"/>
-      <c r="I18" s="38" t="s">
+      <c r="I18" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="38"/>
+      <c r="J18" s="37"/>
       <c r="K18" s="18" t="s">
         <v>18</v>
       </c>
@@ -2209,34 +2266,38 @@
         <v>21</v>
       </c>
       <c r="F19" s="16"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="26" t="str">
+      <c r="G19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="16"/>
+      <c r="I19" s="25" t="str">
         <f aca="false">IF(G19=E19,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J19" s="26"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J19" s="25"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
     </row>
     <row r="20" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
       <c r="C20" s="23"/>
       <c r="D20" s="24"/>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="26" t="str">
+      <c r="F20" s="27"/>
+      <c r="G20" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="27"/>
+      <c r="I20" s="25" t="str">
         <f aca="false">IF(G20=E20,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J20" s="26"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J20" s="25"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
     </row>
     <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="22"/>
@@ -2247,53 +2308,59 @@
         <v>23</v>
       </c>
       <c r="F21" s="16"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="26" t="str">
+      <c r="G21" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="16"/>
+      <c r="I21" s="25" t="str">
         <f aca="false">IF(G21=E21,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J21" s="26"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J21" s="25"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="22"/>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
       <c r="D22" s="24"/>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="26" t="str">
+      <c r="F22" s="27"/>
+      <c r="G22" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="27"/>
+      <c r="I22" s="25" t="str">
         <f aca="false">IF(G22=E22,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J22" s="26"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J22" s="25"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="22"/>
       <c r="B23" s="23"/>
       <c r="C23" s="23"/>
       <c r="D23" s="24"/>
-      <c r="E23" s="28" t="s">
+      <c r="E23" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="28"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="26" t="str">
+      <c r="F23" s="27"/>
+      <c r="G23" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="27"/>
+      <c r="I23" s="25" t="str">
         <f aca="false">IF(G23=E23,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J23" s="26"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J23" s="25"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
     </row>
     <row r="24" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="22" t="n">
@@ -2310,15 +2377,17 @@
         <v>28</v>
       </c>
       <c r="F24" s="23"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="26" t="str">
+      <c r="G24" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="23"/>
+      <c r="I24" s="25" t="str">
         <f aca="false">IF(G24=E24,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J24" s="26"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J24" s="25"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
     </row>
     <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2443,7 +2512,7 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="1" sqref="I6:J11 I19"/>
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2552,10 +2621,10 @@
         <v>16</v>
       </c>
       <c r="H5" s="20"/>
-      <c r="I5" s="38" t="s">
+      <c r="I5" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="38"/>
+      <c r="J5" s="37"/>
       <c r="K5" s="18" t="s">
         <v>18</v>
       </c>
@@ -2576,34 +2645,38 @@
         <v>21</v>
       </c>
       <c r="F6" s="16"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26" t="str">
+      <c r="G6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="I6" s="25" t="str">
         <f aca="false">IF(G6=E6,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J6" s="26"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J6" s="25"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
     </row>
     <row r="7" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="22"/>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
       <c r="D7" s="24"/>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="26" t="str">
+      <c r="F7" s="27"/>
+      <c r="G7" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="27"/>
+      <c r="I7" s="25" t="str">
         <f aca="false">IF(G7=E7,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J7" s="26"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
     </row>
     <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="22"/>
@@ -2614,53 +2687,59 @@
         <v>23</v>
       </c>
       <c r="F8" s="16"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="26" t="str">
+      <c r="G8" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="I8" s="25" t="str">
         <f aca="false">IF(G8=E8,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J8" s="25"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="24"/>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="26" t="str">
+      <c r="F9" s="27"/>
+      <c r="G9" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="27"/>
+      <c r="I9" s="25" t="str">
         <f aca="false">IF(G9=E9,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J9" s="26"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J9" s="25"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="24"/>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="26" t="str">
+      <c r="F10" s="27"/>
+      <c r="G10" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="27"/>
+      <c r="I10" s="25" t="str">
         <f aca="false">IF(G10=E10,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J10" s="26"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J10" s="25"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
     </row>
     <row r="11" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="n">
@@ -2677,15 +2756,17 @@
         <v>28</v>
       </c>
       <c r="F11" s="23"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="26" t="str">
+      <c r="G11" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="23"/>
+      <c r="I11" s="25" t="str">
         <f aca="false">IF(G11=E11,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J11" s="26"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J11" s="25"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9"/>
@@ -2702,64 +2783,64 @@
       <c r="L12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="29"/>
+      <c r="A13" s="28"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="32" t="s">
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="34"/>
+      <c r="H14" s="33"/>
       <c r="I14" s="6"/>
       <c r="J14" s="7"/>
       <c r="L14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31" t="s">
+      <c r="B15" s="29"/>
+      <c r="C15" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="32" t="s">
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="35" t="s">
+      <c r="G15" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="H15" s="35"/>
+      <c r="H15" s="34"/>
       <c r="I15" s="11"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="31" t="s">
+      <c r="B16" s="29"/>
+      <c r="C16" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32" t="s">
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="36"/>
-      <c r="H16" s="37"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="36"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
@@ -2800,10 +2881,10 @@
         <v>16</v>
       </c>
       <c r="H18" s="20"/>
-      <c r="I18" s="38" t="s">
+      <c r="I18" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="38"/>
+      <c r="J18" s="37"/>
       <c r="K18" s="18" t="s">
         <v>18</v>
       </c>
@@ -2824,34 +2905,38 @@
         <v>21</v>
       </c>
       <c r="F19" s="16"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="26" t="str">
+      <c r="G19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="16"/>
+      <c r="I19" s="25" t="str">
         <f aca="false">IF(G19=E19,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J19" s="26"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J19" s="25"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
     </row>
     <row r="20" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
       <c r="C20" s="23"/>
       <c r="D20" s="24"/>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="26" t="str">
+      <c r="F20" s="27"/>
+      <c r="G20" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="27"/>
+      <c r="I20" s="25" t="str">
         <f aca="false">IF(G20=E20,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J20" s="26"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J20" s="25"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
     </row>
     <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="22"/>
@@ -2862,53 +2947,59 @@
         <v>23</v>
       </c>
       <c r="F21" s="16"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="26" t="str">
+      <c r="G21" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="16"/>
+      <c r="I21" s="25" t="str">
         <f aca="false">IF(G21=E21,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J21" s="26"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J21" s="25"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="22"/>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
       <c r="D22" s="24"/>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="26" t="str">
+      <c r="F22" s="27"/>
+      <c r="G22" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="27"/>
+      <c r="I22" s="25" t="str">
         <f aca="false">IF(G22=E22,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J22" s="26"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J22" s="25"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="22"/>
       <c r="B23" s="23"/>
       <c r="C23" s="23"/>
       <c r="D23" s="24"/>
-      <c r="E23" s="28" t="s">
+      <c r="E23" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="28"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="26" t="str">
+      <c r="F23" s="27"/>
+      <c r="G23" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="27"/>
+      <c r="I23" s="25" t="str">
         <f aca="false">IF(G23=E23,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J23" s="26"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J23" s="25"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
     </row>
     <row r="24" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="22" t="n">
@@ -2925,15 +3016,17 @@
         <v>28</v>
       </c>
       <c r="F24" s="23"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="26" t="str">
+      <c r="G24" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="23"/>
+      <c r="I24" s="25" t="str">
         <f aca="false">IF(G24=E24,"Pass","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="J24" s="26"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
+        <v>Pass</v>
+      </c>
+      <c r="J24" s="25"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
     </row>
     <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>